<commit_message>
More unit test, add readstrings tests
</commit_message>
<xml_diff>
--- a/ExcelReader.Test/Files/numbers.xlsx
+++ b/ExcelReader.Test/Files/numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MX05711629\KOF\code\ExcelReader\ExcelReader.Test\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A13D91-267D-47D4-B1BF-D82EAC9F4653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F360E1-B36E-4BF2-9464-A8BC58B5546C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,14 +68,13 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -228,7 +227,7 @@
       <c r="A2">
         <v>13</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2">
         <v>412</v>
       </c>
       <c r="C2" s="1"/>
@@ -240,7 +239,7 @@
       <c r="A3">
         <v>13</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3">
         <v>124</v>
       </c>
       <c r="C3" s="1"/>

</xml_diff>